<commit_message>
Update all files for February 2024 statistics
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2024/2024_99_g_net_borrower_lender.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D53920-2D86-4709-AB59-707E0597953A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9863E270-3EF8-4630-BF67-B269DF62377C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="147">
   <si>
     <t>NET</t>
   </si>
@@ -376,6 +376,123 @@
   </si>
   <si>
     <t>1.51 : 1</t>
+  </si>
+  <si>
+    <t>1.30 : 1</t>
+  </si>
+  <si>
+    <t>0.68 : 1</t>
+  </si>
+  <si>
+    <t>1.06 : 1</t>
+  </si>
+  <si>
+    <t>1.23 : 1</t>
+  </si>
+  <si>
+    <t>2.52 : 1</t>
+  </si>
+  <si>
+    <t>0.41 : 1</t>
+  </si>
+  <si>
+    <t>1.89 : 1</t>
+  </si>
+  <si>
+    <t>0.36 : 1</t>
+  </si>
+  <si>
+    <t>0.93 : 1</t>
+  </si>
+  <si>
+    <t>0.32 : 1</t>
+  </si>
+  <si>
+    <t>0.08 : 1</t>
+  </si>
+  <si>
+    <t>0.18 : 1</t>
+  </si>
+  <si>
+    <t>0.13 : 1</t>
+  </si>
+  <si>
+    <t>1.44 : 1</t>
+  </si>
+  <si>
+    <t>0.48 : 1</t>
+  </si>
+  <si>
+    <t>0.79 : 1</t>
+  </si>
+  <si>
+    <t>1.28 : 1</t>
+  </si>
+  <si>
+    <t>0.92 : 1</t>
+  </si>
+  <si>
+    <t>0.21 : 1</t>
+  </si>
+  <si>
+    <t>6.33 : 1</t>
+  </si>
+  <si>
+    <t>1.45 : 1</t>
+  </si>
+  <si>
+    <t>0.98 : 1</t>
+  </si>
+  <si>
+    <t>0.46 : 1</t>
+  </si>
+  <si>
+    <t>1.64 : 1</t>
+  </si>
+  <si>
+    <t>1.90 : 1</t>
+  </si>
+  <si>
+    <t>0.12 : 1</t>
+  </si>
+  <si>
+    <t>0.01 : 1</t>
+  </si>
+  <si>
+    <t>1.18 : 1</t>
+  </si>
+  <si>
+    <t>0.88 : 1</t>
+  </si>
+  <si>
+    <t>1.35 : 1</t>
+  </si>
+  <si>
+    <t>0.57 : 1</t>
+  </si>
+  <si>
+    <t>1.99 : 1</t>
+  </si>
+  <si>
+    <t>5.73 : 1</t>
+  </si>
+  <si>
+    <t>0.00 : 1</t>
+  </si>
+  <si>
+    <t>0.72 : 1</t>
+  </si>
+  <si>
+    <t>1.38 : 1</t>
+  </si>
+  <si>
+    <t>0.65 : 1</t>
+  </si>
+  <si>
+    <t>0.99 : 1</t>
+  </si>
+  <si>
+    <t>1.10 : 1</t>
   </si>
 </sst>
 </file>
@@ -1285,15 +1402,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>1329</v>
+        <v>2737</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>1284</v>
+        <v>2423</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>45</v>
+        <v>314</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1305,7 +1422,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f t="shared" ref="G2:G33" si="2">IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.04 : 1</v>
+        <v>1.13 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1314,15 +1431,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>534</v>
+        <v>1082</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>401</v>
+        <v>899</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>133</v>
+        <v>183</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1334,7 +1451,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.33 : 1</v>
+        <v>1.2 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1343,15 +1460,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>1209</v>
+        <v>2442</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>1168</v>
+        <v>2408</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1363,7 +1480,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.04 : 1</v>
+        <v>1.01 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1372,15 +1489,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>130</v>
+        <v>233</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-95</v>
+        <v>-143</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1392,7 +1509,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.27 : 1</v>
+        <v>0.39 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1401,15 +1518,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>1109</v>
+        <v>2148</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>1358</v>
+        <v>2945</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-249</v>
+        <v>-797</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1421,7 +1538,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.82 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1430,15 +1547,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>257</v>
+        <v>488</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>133</v>
+        <v>301</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>124</v>
+        <v>187</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1450,7 +1567,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.93 : 1</v>
+        <v>1.62 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1459,15 +1576,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>85</v>
+        <v>222</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-75</v>
+        <v>-138</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1479,7 +1596,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.53 : 1</v>
+        <v>0.62 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1488,15 +1605,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>78</v>
+        <v>156</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-21</v>
+        <v>-43</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1508,7 +1625,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.73 : 1</v>
+        <v>0.72 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1521,11 +1638,11 @@
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-34</v>
+        <v>-91</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1537,7 +1654,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.03 : 1</v>
+        <v>0.01 : 1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1575,27 +1692,27 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>-5</v>
+        <v>66</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>We borrowed more than we lent this year</v>
       </c>
       <c r="F12" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>We lent more than we borrowed this year</v>
+        <v/>
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.81 : 1</v>
+        <v>2.61 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1604,15 +1721,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>170</v>
+        <v>375</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>107</v>
+        <v>210</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>63</v>
+        <v>165</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -1624,7 +1741,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.59 : 1</v>
+        <v>1.79 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1633,15 +1750,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>152</v>
+        <v>283</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>274</v>
+        <v>546</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-122</v>
+        <v>-263</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="0"/>
@@ -1653,7 +1770,7 @@
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.55 : 1</v>
+        <v>0.52 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1662,15 +1779,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>159</v>
+        <v>276</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-93</v>
+        <v>-161</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -1691,15 +1808,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>164</v>
+        <v>308</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-114</v>
+        <v>-176</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1711,7 +1828,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.3 : 1</v>
+        <v>0.43 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1720,15 +1837,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>619</v>
+        <v>1200</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>444</v>
+        <v>873</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>175</v>
+        <v>327</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1740,7 +1857,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.39 : 1</v>
+        <v>1.37 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1749,15 +1866,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>85</v>
+        <v>161</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>98</v>
+        <v>184</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-13</v>
+        <v>-23</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1769,7 +1886,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.87 : 1</v>
+        <v>0.88 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1778,15 +1895,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>615</v>
+        <v>1118</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>429</v>
+        <v>857</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>186</v>
+        <v>261</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1798,7 +1915,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.43 : 1</v>
+        <v>1.3 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1807,15 +1924,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>61</v>
+        <v>180</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-57</v>
+        <v>-175</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1827,7 +1944,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.07 : 1</v>
+        <v>0.03 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1836,15 +1953,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>423</v>
+        <v>837</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>340</v>
+        <v>730</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1856,7 +1973,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.24 : 1</v>
+        <v>1.15 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1865,15 +1982,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>151</v>
+        <v>298</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-135</v>
+        <v>-264</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1894,15 +2011,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>619</v>
+        <v>1263</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>366</v>
+        <v>705</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>253</v>
+        <v>558</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1914,7 +2031,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.69 : 1</v>
+        <v>1.79 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1923,15 +2040,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>1721</v>
+        <v>3610</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>1144</v>
+        <v>2298</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>577</v>
+        <v>1312</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1943,7 +2060,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.5 : 1</v>
+        <v>1.57 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1952,15 +2069,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>158</v>
+        <v>294</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>297</v>
+        <v>591</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-139</v>
+        <v>-297</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1972,7 +2089,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.53 : 1</v>
+        <v>0.5 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2010,15 +2127,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>255</v>
+        <v>456</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>218</v>
+        <v>424</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2030,7 +2147,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.17 : 1</v>
+        <v>1.08 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2039,15 +2156,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>58</v>
+        <v>133</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>113</v>
+        <v>220</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-55</v>
+        <v>-87</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2059,7 +2176,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.51 : 1</v>
+        <v>0.6 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2068,15 +2185,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>528</v>
+        <v>1111</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>422</v>
+        <v>824</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>106</v>
+        <v>287</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2088,7 +2205,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.25 : 1</v>
+        <v>1.35 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2097,15 +2214,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2117,7 +2234,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.95 : 1</v>
+        <v>3.68 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2126,15 +2243,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>302</v>
+        <v>654</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-235</v>
+        <v>-512</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2155,15 +2272,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>361</v>
+        <v>858</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>513</v>
+        <v>1054</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-152</v>
+        <v>-196</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2175,7 +2292,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.7 : 1</v>
+        <v>0.81 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2184,15 +2301,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>336</v>
+        <v>609</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>485</v>
+        <v>1020</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-149</v>
+        <v>-411</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2204,7 +2321,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.69 : 1</v>
+        <v>0.6 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,18 +2330,18 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>147</v>
+        <v>287</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>107</v>
+        <v>216</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="E34" s="28" t="str">
-        <f t="shared" ref="E34:E65" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
+        <f t="shared" ref="E34:E55" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
         <v>We borrowed more than we lent this year</v>
       </c>
       <c r="F34" s="28" t="str">
@@ -2233,7 +2350,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G55" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.37 : 1</v>
+        <v>1.33 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2242,15 +2359,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>787</v>
+        <v>1619</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>1111</v>
+        <v>2159</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-324</v>
+        <v>-540</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2262,7 +2379,7 @@
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.71 : 1</v>
+        <v>0.75 : 1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2271,15 +2388,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>176</v>
+        <v>411</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>410</v>
+        <v>900</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-234</v>
+        <v>-489</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2291,7 +2408,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.43 : 1</v>
+        <v>0.46 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2300,15 +2417,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>450</v>
+        <v>890</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>286</v>
+        <v>592</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>164</v>
+        <v>298</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2320,7 +2437,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.57 : 1</v>
+        <v>1.5 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2329,15 +2446,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>168</v>
+        <v>356</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-143</v>
+        <v>-307</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2349,7 +2466,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.15 : 1</v>
+        <v>0.14 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2358,15 +2475,15 @@
       </c>
       <c r="B39" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="C39" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="D39" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>-12</v>
+        <v>-18</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2378,7 +2495,7 @@
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.8 : 1</v>
+        <v>0.87 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2387,15 +2504,15 @@
       </c>
       <c r="B40" s="8">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C40" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>89</v>
+        <v>203</v>
       </c>
       <c r="D40" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-18</v>
+        <v>-111</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2407,7 +2524,7 @@
       </c>
       <c r="G40" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.8 : 1</v>
+        <v>0.45 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2416,15 +2533,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="C41" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="D41" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2445,15 +2562,15 @@
       </c>
       <c r="B42" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C42" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="D42" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-30</v>
+        <v>-63</v>
       </c>
       <c r="E42" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2465,7 +2582,7 @@
       </c>
       <c r="G42" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.06 : 1</v>
+        <v>0.07 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2474,15 +2591,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C43" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="D43" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-17</v>
+        <v>-42</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2494,7 +2611,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.37 : 1</v>
+        <v>0.34 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2532,15 +2649,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>71</v>
+        <v>137</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>126</v>
+        <v>309</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-55</v>
+        <v>-172</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2552,7 +2669,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.56 : 1</v>
+        <v>0.44 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2561,15 +2678,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>515</v>
+        <v>1123</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>628</v>
+        <v>1210</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-113</v>
+        <v>-87</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2581,7 +2698,7 @@
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.82 : 1</v>
+        <v>0.93 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2590,15 +2707,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>1087</v>
+        <v>2230</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>551</v>
+        <v>1156</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>536</v>
+        <v>1074</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2610,7 +2727,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.97 : 1</v>
+        <v>1.93 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2619,15 +2736,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>264</v>
+        <v>527</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>673</v>
+        <v>1311</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-409</v>
+        <v>-784</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2639,7 +2756,7 @@
       </c>
       <c r="G48" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.39 : 1</v>
+        <v>0.4 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2648,15 +2765,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>513</v>
+        <v>1052</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>251</v>
+        <v>465</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>262</v>
+        <v>587</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2668,7 +2785,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.04 : 1</v>
+        <v>2.26 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2677,15 +2794,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>906</v>
+        <v>1803</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>441</v>
+        <v>972</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>465</v>
+        <v>831</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2697,7 +2814,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>2.05 : 1</v>
+        <v>1.85 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2706,15 +2823,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>187</v>
+        <v>391</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>154</v>
+        <v>320</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2726,7 +2843,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.21 : 1</v>
+        <v>1.22 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2735,15 +2852,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>322</v>
+        <v>689</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>399</v>
+        <v>744</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-77</v>
+        <v>-55</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2755,7 +2872,7 @@
       </c>
       <c r="G52" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.81 : 1</v>
+        <v>0.93 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2764,15 +2881,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>113</v>
+        <v>251</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>218</v>
+        <v>422</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-105</v>
+        <v>-171</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2784,7 +2901,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.52 : 1</v>
+        <v>0.59 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2793,15 +2910,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>207</v>
+        <v>432</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-192</v>
+        <v>-401</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2822,15 +2939,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>300</v>
+        <v>588</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>199</v>
+        <v>420</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>101</v>
+        <v>168</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="3"/>
@@ -2842,7 +2959,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>1.51 : 1</v>
+        <v>1.4 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -6739,108 +6856,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1408</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1139</v>
+      </c>
+      <c r="D2" s="18">
+        <v>269</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>548</v>
+      </c>
+      <c r="C3" s="21">
+        <v>498</v>
+      </c>
+      <c r="D3" s="21">
+        <v>50</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>1233</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1240</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-7</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>55</v>
+      </c>
+      <c r="C5" s="21">
+        <v>103</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-48</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1039</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1587</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-548</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>231</v>
+      </c>
+      <c r="C7" s="21">
+        <v>168</v>
+      </c>
+      <c r="D7" s="21">
+        <v>63</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>137</v>
+      </c>
+      <c r="C8" s="18">
+        <v>200</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-63</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>56</v>
+      </c>
+      <c r="C9" s="21">
+        <v>78</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-22</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>57</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-57</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -6849,163 +7062,309 @@
       <c r="A12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="30"/>
+      <c r="B12" s="23">
+        <v>86</v>
+      </c>
+      <c r="C12" s="23">
+        <v>15</v>
+      </c>
+      <c r="D12" s="23">
+        <v>71</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>205</v>
+      </c>
+      <c r="C13" s="23">
+        <v>103</v>
+      </c>
+      <c r="D13" s="23">
+        <v>102</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>131</v>
+      </c>
+      <c r="C14" s="23">
+        <v>272</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-141</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>49</v>
+      </c>
+      <c r="C15" s="23">
+        <v>117</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-68</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>82</v>
+      </c>
+      <c r="C16" s="18">
+        <v>144</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-62</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>581</v>
+      </c>
+      <c r="C17" s="21">
+        <v>429</v>
+      </c>
+      <c r="D17" s="21">
+        <v>152</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>76</v>
+      </c>
+      <c r="C18" s="18">
+        <v>86</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-10</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>503</v>
+      </c>
+      <c r="C19" s="21">
+        <v>428</v>
+      </c>
+      <c r="D19" s="21">
+        <v>75</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>1</v>
+      </c>
+      <c r="C20" s="18">
+        <v>119</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-118</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>414</v>
+      </c>
+      <c r="C21" s="21">
+        <v>390</v>
+      </c>
+      <c r="D21" s="21">
+        <v>24</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>18</v>
+      </c>
+      <c r="C22" s="18">
+        <v>147</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-129</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>644</v>
+      </c>
+      <c r="C23" s="21">
+        <v>339</v>
+      </c>
+      <c r="D23" s="21">
+        <v>305</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1889</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1154</v>
+      </c>
+      <c r="D24" s="18">
+        <v>735</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>136</v>
+      </c>
+      <c r="C25" s="21">
+        <v>294</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-158</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -7014,185 +7373,351 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
+      <c r="B27" s="21">
+        <v>201</v>
+      </c>
+      <c r="C27" s="21">
+        <v>206</v>
+      </c>
+      <c r="D27" s="21">
+        <v>-5</v>
+      </c>
       <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="F27" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="18">
+        <v>75</v>
+      </c>
+      <c r="C28" s="18">
+        <v>107</v>
+      </c>
+      <c r="D28" s="18">
+        <v>-32</v>
+      </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>583</v>
+      </c>
+      <c r="C29" s="21">
+        <v>402</v>
+      </c>
+      <c r="D29" s="21">
+        <v>181</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="18">
+        <v>38</v>
+      </c>
+      <c r="C30" s="18">
+        <v>6</v>
+      </c>
+      <c r="D30" s="18">
+        <v>32</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>75</v>
+      </c>
+      <c r="C31" s="21">
+        <v>352</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-277</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>497</v>
+      </c>
+      <c r="C32" s="18">
+        <v>541</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-44</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>273</v>
+      </c>
+      <c r="C33" s="21">
+        <v>535</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-262</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>140</v>
+      </c>
+      <c r="C34" s="18">
+        <v>109</v>
+      </c>
+      <c r="D34" s="18">
+        <v>31</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>832</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1048</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-216</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>235</v>
+      </c>
+      <c r="C36" s="18">
+        <v>490</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-255</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>440</v>
+      </c>
+      <c r="C37" s="21">
+        <v>306</v>
+      </c>
+      <c r="D37" s="21">
+        <v>134</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>24</v>
+      </c>
+      <c r="C38" s="18">
+        <v>188</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-164</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>21</v>
+      </c>
+      <c r="C39" s="25">
+        <v>114</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-93</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="31"/>
+      <c r="B40" s="25">
+        <v>96</v>
+      </c>
+      <c r="C40" s="25">
+        <v>92</v>
+      </c>
+      <c r="D40" s="25">
+        <v>4</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>61</v>
+      </c>
       <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="G40" s="9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>3</v>
+      </c>
+      <c r="C41" s="25">
+        <v>36</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-33</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="25">
+        <v>12</v>
+      </c>
+      <c r="C42" s="25">
+        <v>37</v>
+      </c>
+      <c r="D42" s="25">
+        <v>-25</v>
+      </c>
       <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="F42" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0</v>
+      </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="9"/>
@@ -7201,133 +7726,253 @@
       <c r="A44" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="B44" s="21">
+        <v>77</v>
+      </c>
+      <c r="C44" s="21">
+        <v>83</v>
+      </c>
+      <c r="D44" s="21">
+        <v>-6</v>
+      </c>
       <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="F44" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>66</v>
+      </c>
+      <c r="C45" s="18">
+        <v>183</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-117</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="29"/>
+      <c r="B46" s="21">
+        <v>608</v>
+      </c>
+      <c r="C46" s="21">
+        <v>582</v>
+      </c>
+      <c r="D46" s="21">
+        <v>26</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="G46" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>1143</v>
+      </c>
+      <c r="C47" s="18">
+        <v>605</v>
+      </c>
+      <c r="D47" s="18">
+        <v>538</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>263</v>
+      </c>
+      <c r="C48" s="21">
+        <v>638</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-375</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>539</v>
+      </c>
+      <c r="C49" s="18">
+        <v>214</v>
+      </c>
+      <c r="D49" s="18">
+        <v>325</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>897</v>
+      </c>
+      <c r="C50" s="21">
+        <v>531</v>
+      </c>
+      <c r="D50" s="21">
+        <v>366</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="18">
+        <v>204</v>
+      </c>
+      <c r="C51" s="18">
+        <v>166</v>
+      </c>
+      <c r="D51" s="18">
+        <v>38</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="29"/>
+      <c r="B52" s="21">
+        <v>367</v>
+      </c>
+      <c r="C52" s="21">
+        <v>345</v>
+      </c>
+      <c r="D52" s="21">
+        <v>22</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="G52" s="5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="18">
+        <v>138</v>
+      </c>
+      <c r="C53" s="18">
+        <v>204</v>
+      </c>
+      <c r="D53" s="18">
+        <v>-66</v>
+      </c>
       <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>16</v>
+      </c>
+      <c r="C54" s="21">
+        <v>225</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-209</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="27">
+        <v>288</v>
+      </c>
+      <c r="C55" s="27">
+        <v>221</v>
+      </c>
+      <c r="D55" s="27">
+        <v>67</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-000002000000}"/>

</xml_diff>

<commit_message>
Update statistics for June, 2024
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2024/2024_99_g_net_borrower_lender.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7A168D-AFD4-4440-93BE-A24C631B976E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734E8F59-7D80-4CDA-A48C-53D6E1A327F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly totals" sheetId="1" r:id="rId1"/>
@@ -47,12 +47,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="226">
   <si>
     <t>NET</t>
   </si>
@@ -691,6 +700,45 @@
   </si>
   <si>
     <t>1.85 : 1</t>
+  </si>
+  <si>
+    <t>1.19 : 1</t>
+  </si>
+  <si>
+    <t>0.26 : 1</t>
+  </si>
+  <si>
+    <t>2.25 : 1</t>
+  </si>
+  <si>
+    <t>0.61 : 1</t>
+  </si>
+  <si>
+    <t>1.34 : 1</t>
+  </si>
+  <si>
+    <t>1.79 : 1</t>
+  </si>
+  <si>
+    <t>0.67 : 1</t>
+  </si>
+  <si>
+    <t>2.51 : 1</t>
+  </si>
+  <si>
+    <t>1.86 : 1</t>
+  </si>
+  <si>
+    <t>0.85 : 1</t>
+  </si>
+  <si>
+    <t>1.83 : 1</t>
+  </si>
+  <si>
+    <t>1.26 : 1</t>
+  </si>
+  <si>
+    <t>2.11 : 1</t>
   </si>
 </sst>
 </file>
@@ -1554,7 +1602,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:XFD1048576"/>
       <selection pane="topRight" sqref="A1:XFD1048576"/>
@@ -1600,15 +1648,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>6773</v>
+        <v>8140</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>5904</v>
+        <v>7055</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>869</v>
+        <v>1085</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1629,15 +1677,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>2848</v>
+        <v>3496</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>2252</v>
+        <v>2622</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>596</v>
+        <v>874</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1649,7 +1697,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.26 : 1</v>
+        <v>1.33 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1658,15 +1706,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>6005</v>
+        <v>7125</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>6113</v>
+        <v>7127</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>-108</v>
+        <v>-2</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1678,7 +1726,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.98 : 1</v>
+        <v>1 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1687,15 +1735,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>197</v>
+        <v>241</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>585</v>
+        <v>756</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-388</v>
+        <v>-515</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1707,7 +1755,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.34 : 1</v>
+        <v>0.32 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1716,15 +1764,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>5389</v>
+        <v>6397</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>7007</v>
+        <v>8396</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-1618</v>
+        <v>-1999</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1736,7 +1784,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.77 : 1</v>
+        <v>0.76 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1745,15 +1793,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>1611</v>
+        <v>1870</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>713</v>
+        <v>866</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>898</v>
+        <v>1004</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1765,7 +1813,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>2.26 : 1</v>
+        <v>2.16 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1774,15 +1822,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>585</v>
+        <v>762</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>907</v>
+        <v>1112</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-322</v>
+        <v>-350</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1794,7 +1842,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.64 : 1</v>
+        <v>0.69 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1803,15 +1851,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>250</v>
+        <v>295</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>368</v>
+        <v>437</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-118</v>
+        <v>-142</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1832,15 +1880,15 @@
       </c>
       <c r="B10" s="2">
         <f>January!B10+February!B10+March!B10+April!B10+May!B10+June!B10+July!B10+August!B10+September!B10+October!B10+November!B10+December!B10</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>258</v>
+        <v>296</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-256</v>
+        <v>-287</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1852,7 +1900,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.01 : 1</v>
+        <v>0.03 : 1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1890,15 +1938,15 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="0"/>
@@ -1910,7 +1958,7 @@
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.54 : 1</v>
+        <v>1.63 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1919,15 +1967,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>826</v>
+        <v>967</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>448</v>
+        <v>534</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>378</v>
+        <v>433</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -1939,7 +1987,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.84 : 1</v>
+        <v>1.81 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1948,15 +1996,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>714</v>
+        <v>811</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>1302</v>
+        <v>1544</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-588</v>
+        <v>-733</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="0"/>
@@ -1968,7 +2016,7 @@
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.55 : 1</v>
+        <v>0.53 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1977,15 +2025,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>281</v>
+        <v>363</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>643</v>
+        <v>777</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-362</v>
+        <v>-414</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -1997,7 +2045,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.44 : 1</v>
+        <v>0.47 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2006,15 +2054,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>344</v>
+        <v>409</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>692</v>
+        <v>839</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-348</v>
+        <v>-430</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2026,7 +2074,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.5 : 1</v>
+        <v>0.49 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2035,15 +2083,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>2932</v>
+        <v>3505</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>2053</v>
+        <v>2519</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>879</v>
+        <v>986</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2055,7 +2103,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.43 : 1</v>
+        <v>1.39 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2064,15 +2112,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>372</v>
+        <v>443</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>496</v>
+        <v>622</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-124</v>
+        <v>-179</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2084,7 +2132,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.75 : 1</v>
+        <v>0.71 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2093,15 +2141,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>2827</v>
+        <v>3309</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>2256</v>
+        <v>2615</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>571</v>
+        <v>694</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2113,7 +2161,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.25 : 1</v>
+        <v>1.27 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2122,15 +2170,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>407</v>
+        <v>466</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-395</v>
+        <v>-453</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2151,15 +2199,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>2128</v>
+        <v>2768</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>1769</v>
+        <v>2126</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>359</v>
+        <v>642</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2171,7 +2219,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.2 : 1</v>
+        <v>1.3 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2180,15 +2228,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>653</v>
+        <v>735</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-533</v>
+        <v>-592</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2200,7 +2248,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.18 : 1</v>
+        <v>0.19 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2209,15 +2257,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>3160</v>
+        <v>3828</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>1721</v>
+        <v>2094</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>1439</v>
+        <v>1734</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2229,7 +2277,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.84 : 1</v>
+        <v>1.83 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2238,15 +2286,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>8952</v>
+        <v>10290</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>6064</v>
+        <v>7338</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>2888</v>
+        <v>2952</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2258,7 +2306,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.48 : 1</v>
+        <v>1.4 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2267,15 +2315,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>727</v>
+        <v>909</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>1571</v>
+        <v>1941</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-844</v>
+        <v>-1032</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2287,7 +2335,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.46 : 1</v>
+        <v>0.47 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2325,15 +2373,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>1197</v>
+        <v>1474</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>961</v>
+        <v>1150</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>236</v>
+        <v>324</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2345,7 +2393,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.25 : 1</v>
+        <v>1.28 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2354,15 +2402,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>389</v>
+        <v>450</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>491</v>
+        <v>587</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-102</v>
+        <v>-137</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2374,7 +2422,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.79 : 1</v>
+        <v>0.77 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2383,15 +2431,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>2811</v>
+        <v>3205</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>2029</v>
+        <v>2454</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>782</v>
+        <v>751</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2403,7 +2451,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.39 : 1</v>
+        <v>1.31 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2412,15 +2460,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>251</v>
+        <v>295</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2432,7 +2480,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.15 : 1</v>
+        <v>2.06 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2441,15 +2489,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>310</v>
+        <v>342</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>1506</v>
+        <v>1764</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-1196</v>
+        <v>-1422</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2461,7 +2509,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.21 : 1</v>
+        <v>0.19 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2470,15 +2518,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>2155</v>
+        <v>2563</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>2655</v>
+        <v>3266</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-500</v>
+        <v>-703</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2490,7 +2538,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.81 : 1</v>
+        <v>0.78 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2499,15 +2547,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>1555</v>
+        <v>1940</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>2761</v>
+        <v>3326</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-1206</v>
+        <v>-1386</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2519,7 +2567,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.56 : 1</v>
+        <v>0.58 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2528,15 +2576,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>786</v>
+        <v>972</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>489</v>
+        <v>563</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>297</v>
+        <v>409</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E55" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -2548,7 +2596,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G55" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.61 : 1</v>
+        <v>1.73 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2557,15 +2605,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>4063</v>
+        <v>4825</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>5511</v>
+        <v>6513</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-1448</v>
+        <v>-1688</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2586,15 +2634,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>965</v>
+        <v>1188</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>2245</v>
+        <v>2698</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-1280</v>
+        <v>-1510</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2606,7 +2654,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.43 : 1</v>
+        <v>0.44 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2615,15 +2663,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>2265</v>
+        <v>2759</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>1575</v>
+        <v>1840</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>690</v>
+        <v>919</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2635,7 +2683,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.44 : 1</v>
+        <v>1.5 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2644,15 +2692,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>902</v>
+        <v>1086</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-760</v>
+        <v>-909</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2673,15 +2721,15 @@
       </c>
       <c r="B39" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>433</v>
+        <v>487</v>
       </c>
       <c r="C39" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>394</v>
+        <v>467</v>
       </c>
       <c r="D39" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2693,7 +2741,7 @@
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.1 : 1</v>
+        <v>1.04 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2706,11 +2754,11 @@
       </c>
       <c r="C40" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="D40" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-360</v>
+        <v>-370</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2722,7 +2770,7 @@
       </c>
       <c r="G40" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.25 : 1</v>
+        <v>0.24 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2735,11 +2783,11 @@
       </c>
       <c r="C41" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>475</v>
+        <v>484</v>
       </c>
       <c r="D41" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-110</v>
+        <v>-119</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2751,7 +2799,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.77 : 1</v>
+        <v>0.75 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2764,11 +2812,11 @@
       </c>
       <c r="C42" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D42" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-169</v>
+        <v>-171</v>
       </c>
       <c r="E42" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2793,11 +2841,11 @@
       </c>
       <c r="C43" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D43" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-81</v>
+        <v>-83</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2809,7 +2857,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.34 : 1</v>
+        <v>0.33 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2847,15 +2895,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>346</v>
+        <v>437</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>874</v>
+        <v>1063</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-528</v>
+        <v>-626</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2867,7 +2915,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.4 : 1</v>
+        <v>0.41 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2876,15 +2924,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>2529</v>
+        <v>2974</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>2964</v>
+        <v>3488</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-435</v>
+        <v>-514</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2905,15 +2953,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>5285</v>
+        <v>6319</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>2892</v>
+        <v>3417</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>2393</v>
+        <v>2902</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2925,7 +2973,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.83 : 1</v>
+        <v>1.85 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2934,15 +2982,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>1322</v>
+        <v>1537</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>2921</v>
+        <v>3418</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-1599</v>
+        <v>-1881</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2963,15 +3011,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>2613</v>
+        <v>3117</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>1203</v>
+        <v>1479</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>1410</v>
+        <v>1638</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2983,7 +3031,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.17 : 1</v>
+        <v>2.11 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2992,15 +3040,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>4616</v>
+        <v>5585</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>2624</v>
+        <v>3232</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>1992</v>
+        <v>2353</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3012,7 +3060,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.76 : 1</v>
+        <v>1.73 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3021,15 +3069,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>1036</v>
+        <v>1239</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>866</v>
+        <v>1027</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3041,7 +3089,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.2 : 1</v>
+        <v>1.21 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3050,15 +3098,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>1732</v>
+        <v>2052</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>2000</v>
+        <v>2407</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-268</v>
+        <v>-355</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3070,7 +3118,7 @@
       </c>
       <c r="G52" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.87 : 1</v>
+        <v>0.85 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3079,15 +3127,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>608</v>
+        <v>711</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>1093</v>
+        <v>1330</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-485</v>
+        <v>-619</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3099,7 +3147,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.56 : 1</v>
+        <v>0.53 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3108,15 +3156,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>1071</v>
+        <v>1284</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-981</v>
+        <v>-1166</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3128,7 +3176,7 @@
       </c>
       <c r="G54" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.08 : 1</v>
+        <v>0.09 : 1</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3137,15 +3185,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>1467</v>
+        <v>1830</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>1034</v>
+        <v>1206</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>433</v>
+        <v>624</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3157,7 +3205,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>1.42 : 1</v>
+        <v>1.52 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -11763,7 +11811,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -11807,108 +11855,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1367</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1151</v>
+      </c>
+      <c r="D2" s="18">
+        <v>216</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>648</v>
+      </c>
+      <c r="C3" s="21">
+        <v>370</v>
+      </c>
+      <c r="D3" s="21">
+        <v>278</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="18">
+        <v>1120</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1014</v>
+      </c>
+      <c r="D4" s="18">
+        <v>106</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>44</v>
+      </c>
+      <c r="C5" s="21">
+        <v>171</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-127</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1008</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1389</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-381</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>259</v>
+      </c>
+      <c r="C7" s="21">
+        <v>153</v>
+      </c>
+      <c r="D7" s="21">
+        <v>106</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>177</v>
+      </c>
+      <c r="C8" s="18">
+        <v>205</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-28</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>45</v>
+      </c>
+      <c r="C9" s="21">
+        <v>69</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-24</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18">
+        <v>38</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-31</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -11917,163 +12061,309 @@
       <c r="A12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="30"/>
+      <c r="B12" s="23">
+        <v>36</v>
+      </c>
+      <c r="C12" s="23">
+        <v>16</v>
+      </c>
+      <c r="D12" s="23">
+        <v>20</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>141</v>
+      </c>
+      <c r="C13" s="23">
+        <v>86</v>
+      </c>
+      <c r="D13" s="23">
+        <v>55</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>97</v>
+      </c>
+      <c r="C14" s="23">
+        <v>242</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-145</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>82</v>
+      </c>
+      <c r="C15" s="23">
+        <v>134</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-52</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>65</v>
+      </c>
+      <c r="C16" s="18">
+        <v>147</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-82</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>573</v>
+      </c>
+      <c r="C17" s="21">
+        <v>466</v>
+      </c>
+      <c r="D17" s="21">
+        <v>107</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>71</v>
+      </c>
+      <c r="C18" s="18">
+        <v>126</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-55</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>482</v>
+      </c>
+      <c r="C19" s="21">
+        <v>359</v>
+      </c>
+      <c r="D19" s="21">
+        <v>123</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>1</v>
+      </c>
+      <c r="C20" s="18">
+        <v>59</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-58</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>640</v>
+      </c>
+      <c r="C21" s="21">
+        <v>357</v>
+      </c>
+      <c r="D21" s="21">
+        <v>283</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>23</v>
+      </c>
+      <c r="C22" s="18">
+        <v>82</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-59</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>668</v>
+      </c>
+      <c r="C23" s="21">
+        <v>373</v>
+      </c>
+      <c r="D23" s="21">
+        <v>295</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1338</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1274</v>
+      </c>
+      <c r="D24" s="18">
+        <v>64</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>182</v>
+      </c>
+      <c r="C25" s="21">
+        <v>370</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-188</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -12082,185 +12372,351 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>277</v>
+      </c>
+      <c r="C27" s="21">
+        <v>189</v>
+      </c>
+      <c r="D27" s="21">
+        <v>88</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="18">
+        <v>61</v>
+      </c>
+      <c r="C28" s="18">
+        <v>96</v>
+      </c>
+      <c r="D28" s="18">
+        <v>-35</v>
+      </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
+      <c r="B29" s="21">
+        <v>394</v>
+      </c>
+      <c r="C29" s="21">
+        <v>425</v>
+      </c>
+      <c r="D29" s="21">
+        <v>-31</v>
+      </c>
       <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="F29" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="18">
+        <v>44</v>
+      </c>
+      <c r="C30" s="18">
+        <v>26</v>
+      </c>
+      <c r="D30" s="18">
+        <v>18</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>32</v>
+      </c>
+      <c r="C31" s="21">
+        <v>258</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-226</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>408</v>
+      </c>
+      <c r="C32" s="18">
+        <v>611</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-203</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>385</v>
+      </c>
+      <c r="C33" s="21">
+        <v>565</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-180</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>186</v>
+      </c>
+      <c r="C34" s="18">
+        <v>74</v>
+      </c>
+      <c r="D34" s="18">
+        <v>112</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>762</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1002</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-240</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>223</v>
+      </c>
+      <c r="C36" s="18">
+        <v>453</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-230</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>494</v>
+      </c>
+      <c r="C37" s="21">
+        <v>265</v>
+      </c>
+      <c r="D37" s="21">
+        <v>229</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>35</v>
+      </c>
+      <c r="C38" s="18">
+        <v>184</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-149</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>0</v>
+      </c>
+      <c r="C39" s="25">
+        <v>10</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-10</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="25">
+        <v>0</v>
+      </c>
+      <c r="C40" s="25">
+        <v>9</v>
+      </c>
+      <c r="D40" s="25">
+        <v>-9</v>
+      </c>
       <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="F40" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>0</v>
+      </c>
+      <c r="C41" s="25">
+        <v>2</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-2</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="25">
+        <v>0</v>
+      </c>
+      <c r="C42" s="25">
+        <v>2</v>
+      </c>
+      <c r="D42" s="25">
+        <v>-2</v>
+      </c>
       <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="F42" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0</v>
+      </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="9"/>
@@ -12269,133 +12725,253 @@
       <c r="A44" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="B44" s="21">
+        <v>54</v>
+      </c>
+      <c r="C44" s="21">
+        <v>73</v>
+      </c>
+      <c r="D44" s="21">
+        <v>-19</v>
+      </c>
       <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="F44" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>91</v>
+      </c>
+      <c r="C45" s="18">
+        <v>189</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-98</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="B46" s="21">
+        <v>445</v>
+      </c>
+      <c r="C46" s="21">
+        <v>524</v>
+      </c>
+      <c r="D46" s="21">
+        <v>-79</v>
+      </c>
       <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="F46" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>1034</v>
+      </c>
+      <c r="C47" s="18">
+        <v>525</v>
+      </c>
+      <c r="D47" s="18">
+        <v>509</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>215</v>
+      </c>
+      <c r="C48" s="21">
+        <v>497</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-282</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>504</v>
+      </c>
+      <c r="C49" s="18">
+        <v>276</v>
+      </c>
+      <c r="D49" s="18">
+        <v>228</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>969</v>
+      </c>
+      <c r="C50" s="21">
+        <v>608</v>
+      </c>
+      <c r="D50" s="21">
+        <v>361</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="18">
+        <v>203</v>
+      </c>
+      <c r="C51" s="18">
+        <v>161</v>
+      </c>
+      <c r="D51" s="18">
+        <v>42</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="B52" s="21">
+        <v>320</v>
+      </c>
+      <c r="C52" s="21">
+        <v>407</v>
+      </c>
+      <c r="D52" s="21">
+        <v>-87</v>
+      </c>
       <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="18">
+        <v>103</v>
+      </c>
+      <c r="C53" s="18">
+        <v>237</v>
+      </c>
+      <c r="D53" s="18">
+        <v>-134</v>
+      </c>
       <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>28</v>
+      </c>
+      <c r="C54" s="21">
+        <v>213</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-185</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="27">
+        <v>363</v>
+      </c>
+      <c r="C55" s="27">
+        <v>172</v>
+      </c>
+      <c r="D55" s="27">
+        <v>191</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>225</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-000006000000}"/>

</xml_diff>

<commit_message>
Updated statistics and images for October, 2024
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2024/2024_99_g_net_borrower_lender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9588CF81-CE57-41FA-8B90-DA1333C39480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DFBEBF-063E-4058-9F3B-639F86FC816A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="264">
   <si>
     <t>NET</t>
   </si>
@@ -838,6 +838,21 @@
   </si>
   <si>
     <t>0.20 : 1</t>
+  </si>
+  <si>
+    <t>1.71 : 1</t>
+  </si>
+  <si>
+    <t>0.58 : 1</t>
+  </si>
+  <si>
+    <t>1.00 : 1</t>
+  </si>
+  <si>
+    <t>2.30 : 1</t>
+  </si>
+  <si>
+    <t>2.08 : 1</t>
   </si>
 </sst>
 </file>
@@ -1747,15 +1762,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>12673</v>
+        <v>14389</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>10836</v>
+        <v>12130</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>1837</v>
+        <v>2259</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1767,7 +1782,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f t="shared" ref="G2:G33" si="2">IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.17 : 1</v>
+        <v>1.19 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1776,15 +1791,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>5634</v>
+        <v>6346</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>3916</v>
+        <v>4332</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>1718</v>
+        <v>2014</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1796,7 +1811,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.44 : 1</v>
+        <v>1.46 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1805,27 +1820,27 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>10582</v>
+        <v>11795</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>10508</v>
+        <v>11967</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>74</v>
+        <v>-172</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F4" s="28" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.01 : 1</v>
+        <v>0.99 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1834,15 +1849,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>401</v>
+        <v>434</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>1122</v>
+        <v>1279</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-721</v>
+        <v>-845</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1854,7 +1869,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.36 : 1</v>
+        <v>0.34 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1863,15 +1878,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>9478</v>
+        <v>10736</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>12797</v>
+        <v>14346</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-3319</v>
+        <v>-3610</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1883,7 +1898,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.74 : 1</v>
+        <v>0.75 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1892,15 +1907,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>2597</v>
+        <v>2772</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>1484</v>
+        <v>1675</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>1113</v>
+        <v>1097</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1912,7 +1927,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.75 : 1</v>
+        <v>1.65 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1921,15 +1936,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>1157</v>
+        <v>1338</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>1698</v>
+        <v>1905</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-541</v>
+        <v>-567</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1941,7 +1956,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.68 : 1</v>
+        <v>0.7 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1950,15 +1965,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>393</v>
+        <v>448</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>632</v>
+        <v>709</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-239</v>
+        <v>-261</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1970,7 +1985,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.62 : 1</v>
+        <v>0.63 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1983,11 +1998,11 @@
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>461</v>
+        <v>503</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-442</v>
+        <v>-484</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2037,15 +2052,15 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>312</v>
+        <v>329</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2057,7 +2072,7 @@
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.64 : 1</v>
+        <v>1.63 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2066,15 +2081,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>1319</v>
+        <v>1430</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>750</v>
+        <v>825</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>569</v>
+        <v>605</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2086,7 +2101,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.76 : 1</v>
+        <v>1.73 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2095,15 +2110,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>1204</v>
+        <v>1396</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>2286</v>
+        <v>2521</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-1082</v>
+        <v>-1125</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2115,7 +2130,7 @@
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.53 : 1</v>
+        <v>0.55 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2124,15 +2139,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>558</v>
+        <v>613</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>1253</v>
+        <v>1424</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-695</v>
+        <v>-811</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2144,7 +2159,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.45 : 1</v>
+        <v>0.43 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2153,15 +2168,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>569</v>
+        <v>607</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1329</v>
+        <v>1463</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-760</v>
+        <v>-856</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2173,7 +2188,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.43 : 1</v>
+        <v>0.41 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2182,15 +2197,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>5369</v>
+        <v>6070</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>3766</v>
+        <v>4200</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>1603</v>
+        <v>1870</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2202,7 +2217,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.43 : 1</v>
+        <v>1.45 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2211,15 +2226,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>678</v>
+        <v>771</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>921</v>
+        <v>1081</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-243</v>
+        <v>-310</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2231,7 +2246,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.74 : 1</v>
+        <v>0.71 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2240,15 +2255,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>4836</v>
+        <v>5451</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>3951</v>
+        <v>4406</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>885</v>
+        <v>1045</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2260,7 +2275,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.22 : 1</v>
+        <v>1.24 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2269,15 +2284,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>673</v>
+        <v>742</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-587</v>
+        <v>-607</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2289,7 +2304,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.13 : 1</v>
+        <v>0.18 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2298,15 +2313,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>4409</v>
+        <v>4966</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>3160</v>
+        <v>3521</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>1249</v>
+        <v>1445</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2318,7 +2333,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.4 : 1</v>
+        <v>1.41 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2327,15 +2342,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>234</v>
+        <v>287</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>1016</v>
+        <v>1118</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-782</v>
+        <v>-831</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2347,7 +2362,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.23 : 1</v>
+        <v>0.26 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2356,15 +2371,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>5907</v>
+        <v>6542</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>3219</v>
+        <v>3563</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>2688</v>
+        <v>2979</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2385,15 +2400,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>15035</v>
+        <v>16658</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>10791</v>
+        <v>11993</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>4244</v>
+        <v>4665</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2414,15 +2429,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>1305</v>
+        <v>1474</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>3341</v>
+        <v>3875</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-2036</v>
+        <v>-2401</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2434,7 +2449,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.39 : 1</v>
+        <v>0.38 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2472,15 +2487,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>2161</v>
+        <v>2413</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>1798</v>
+        <v>2019</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>363</v>
+        <v>394</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2501,15 +2516,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>741</v>
+        <v>892</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>865</v>
+        <v>955</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-124</v>
+        <v>-63</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2521,7 +2536,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.86 : 1</v>
+        <v>0.93 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2530,15 +2545,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>4845</v>
+        <v>5546</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>3788</v>
+        <v>4259</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>1057</v>
+        <v>1287</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2550,7 +2565,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.28 : 1</v>
+        <v>1.3 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2559,15 +2574,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>383</v>
+        <v>438</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>191</v>
+        <v>224</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2579,7 +2594,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2.01 : 1</v>
+        <v>1.96 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2588,15 +2603,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>472</v>
+        <v>553</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>2617</v>
+        <v>2903</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-2145</v>
+        <v>-2350</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2608,7 +2623,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.18 : 1</v>
+        <v>0.19 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2617,15 +2632,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>3851</v>
+        <v>4294</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>5030</v>
+        <v>5640</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-1179</v>
+        <v>-1346</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2637,7 +2652,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.77 : 1</v>
+        <v>0.76 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2646,15 +2661,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>3200</v>
+        <v>3567</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>5105</v>
+        <v>5617</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-1905</v>
+        <v>-2050</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2666,7 +2681,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.63 : 1</v>
+        <v>0.64 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2675,15 +2690,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>1575</v>
+        <v>1760</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>906</v>
+        <v>1043</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>669</v>
+        <v>717</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E55" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -2695,7 +2710,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G55" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.74 : 1</v>
+        <v>1.69 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2704,15 +2719,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>7599</v>
+        <v>8509</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>10080</v>
+        <v>11380</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-2481</v>
+        <v>-2871</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2733,15 +2748,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>1746</v>
+        <v>1932</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>4274</v>
+        <v>4846</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-2528</v>
+        <v>-2914</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2753,7 +2768,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.41 : 1</v>
+        <v>0.4 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2762,15 +2777,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>4273</v>
+        <v>4888</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>2967</v>
+        <v>3456</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1306</v>
+        <v>1432</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2782,7 +2797,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.44 : 1</v>
+        <v>1.41 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2791,15 +2806,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>251</v>
+        <v>297</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>1584</v>
+        <v>1770</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-1333</v>
+        <v>-1473</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2811,7 +2826,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.16 : 1</v>
+        <v>0.17 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2820,23 +2835,23 @@
       </c>
       <c r="B39" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>698</v>
+        <v>796</v>
       </c>
       <c r="C39" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>696</v>
+        <v>799</v>
       </c>
       <c r="D39" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F39" s="29" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2849,15 +2864,15 @@
       </c>
       <c r="B40" s="8">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>195</v>
+        <v>230</v>
       </c>
       <c r="C40" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>633</v>
+        <v>742</v>
       </c>
       <c r="D40" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-438</v>
+        <v>-512</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2878,15 +2893,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>406</v>
+        <v>465</v>
       </c>
       <c r="C41" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>678</v>
+        <v>825</v>
       </c>
       <c r="D41" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-272</v>
+        <v>-360</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2898,7 +2913,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.6 : 1</v>
+        <v>0.56 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2907,15 +2922,15 @@
       </c>
       <c r="B42" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C42" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>236</v>
+        <v>277</v>
       </c>
       <c r="D42" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-192</v>
+        <v>-213</v>
       </c>
       <c r="E42" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2927,7 +2942,7 @@
       </c>
       <c r="G42" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.19 : 1</v>
+        <v>0.23 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2936,15 +2951,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C43" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="D43" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-133</v>
+        <v>-181</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2956,7 +2971,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.27 : 1</v>
+        <v>0.24 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2994,15 +3009,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>729</v>
+        <v>772</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>1581</v>
+        <v>1775</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-852</v>
+        <v>-1003</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3014,7 +3029,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.46 : 1</v>
+        <v>0.43 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3023,15 +3038,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>4641</v>
+        <v>5267</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>5201</v>
+        <v>5825</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-560</v>
+        <v>-558</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3043,7 +3058,7 @@
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.89 : 1</v>
+        <v>0.9 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3052,15 +3067,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>9420</v>
+        <v>10574</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>5186</v>
+        <v>5821</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>4234</v>
+        <v>4753</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3081,15 +3096,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>2253</v>
+        <v>2495</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>5186</v>
+        <v>5804</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-2933</v>
+        <v>-3309</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3110,15 +3125,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>5055</v>
+        <v>5676</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>2343</v>
+        <v>2613</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>2712</v>
+        <v>3063</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3130,7 +3145,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.16 : 1</v>
+        <v>2.17 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3139,15 +3154,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>8437</v>
+        <v>9244</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>5065</v>
+        <v>5630</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>3372</v>
+        <v>3614</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3159,7 +3174,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.67 : 1</v>
+        <v>1.64 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3168,15 +3183,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>1946</v>
+        <v>2214</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>1484</v>
+        <v>1651</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>462</v>
+        <v>563</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3188,7 +3203,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.31 : 1</v>
+        <v>1.34 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3197,15 +3212,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>3167</v>
+        <v>3541</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>3603</v>
+        <v>4052</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-436</v>
+        <v>-511</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3217,7 +3232,7 @@
       </c>
       <c r="G52" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.88 : 1</v>
+        <v>0.87 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3226,15 +3241,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>1168</v>
+        <v>1371</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>2055</v>
+        <v>2296</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-887</v>
+        <v>-925</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3246,7 +3261,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.57 : 1</v>
+        <v>0.6 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3255,15 +3270,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>233</v>
+        <v>284</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>1954</v>
+        <v>2211</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-1721</v>
+        <v>-1927</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3275,7 +3290,7 @@
       </c>
       <c r="G54" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.12 : 1</v>
+        <v>0.13 : 1</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3284,15 +3299,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>2861</v>
+        <v>3268</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>1764</v>
+        <v>1960</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>1097</v>
+        <v>1308</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3304,7 +3319,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>1.62 : 1</v>
+        <v>1.67 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -4561,108 +4576,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1716</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1294</v>
+      </c>
+      <c r="D2" s="18">
+        <v>422</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>712</v>
+      </c>
+      <c r="C3" s="21">
+        <v>416</v>
+      </c>
+      <c r="D3" s="21">
+        <v>296</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>1213</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1459</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-246</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>33</v>
+      </c>
+      <c r="C5" s="21">
+        <v>157</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-124</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1258</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1549</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-291</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="B7" s="21">
+        <v>175</v>
+      </c>
+      <c r="C7" s="21">
+        <v>191</v>
+      </c>
+      <c r="D7" s="21">
+        <v>-16</v>
+      </c>
       <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>181</v>
+      </c>
+      <c r="C8" s="18">
+        <v>207</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-26</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>55</v>
+      </c>
+      <c r="C9" s="21">
+        <v>77</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-22</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>42</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-42</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -4671,163 +4782,309 @@
       <c r="A12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="30"/>
+      <c r="B12" s="23">
+        <v>17</v>
+      </c>
+      <c r="C12" s="23">
+        <v>12</v>
+      </c>
+      <c r="D12" s="23">
+        <v>5</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>111</v>
+      </c>
+      <c r="C13" s="23">
+        <v>75</v>
+      </c>
+      <c r="D13" s="23">
+        <v>36</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>192</v>
+      </c>
+      <c r="C14" s="23">
+        <v>235</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-43</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>55</v>
+      </c>
+      <c r="C15" s="23">
+        <v>171</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-116</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>38</v>
+      </c>
+      <c r="C16" s="18">
+        <v>134</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-96</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>701</v>
+      </c>
+      <c r="C17" s="21">
+        <v>434</v>
+      </c>
+      <c r="D17" s="21">
+        <v>267</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>93</v>
+      </c>
+      <c r="C18" s="18">
+        <v>160</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-67</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>615</v>
+      </c>
+      <c r="C19" s="21">
+        <v>455</v>
+      </c>
+      <c r="D19" s="21">
+        <v>160</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>49</v>
+      </c>
+      <c r="C20" s="18">
+        <v>69</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-20</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>557</v>
+      </c>
+      <c r="C21" s="21">
+        <v>361</v>
+      </c>
+      <c r="D21" s="21">
+        <v>196</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>53</v>
+      </c>
+      <c r="C22" s="18">
+        <v>102</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-49</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>635</v>
+      </c>
+      <c r="C23" s="21">
+        <v>344</v>
+      </c>
+      <c r="D23" s="21">
+        <v>291</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1623</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1202</v>
+      </c>
+      <c r="D24" s="18">
+        <v>421</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>169</v>
+      </c>
+      <c r="C25" s="21">
+        <v>534</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-365</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -4836,185 +5093,351 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>252</v>
+      </c>
+      <c r="C27" s="21">
+        <v>221</v>
+      </c>
+      <c r="D27" s="21">
+        <v>31</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="18">
+        <v>151</v>
+      </c>
+      <c r="C28" s="18">
+        <v>90</v>
+      </c>
+      <c r="D28" s="18">
+        <v>61</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>701</v>
+      </c>
+      <c r="C29" s="21">
+        <v>471</v>
+      </c>
+      <c r="D29" s="21">
+        <v>230</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="18">
+        <v>55</v>
+      </c>
+      <c r="C30" s="18">
+        <v>33</v>
+      </c>
+      <c r="D30" s="18">
+        <v>22</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>81</v>
+      </c>
+      <c r="C31" s="21">
+        <v>286</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-205</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>443</v>
+      </c>
+      <c r="C32" s="18">
+        <v>610</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-167</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>367</v>
+      </c>
+      <c r="C33" s="21">
+        <v>512</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-145</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>185</v>
+      </c>
+      <c r="C34" s="18">
+        <v>137</v>
+      </c>
+      <c r="D34" s="18">
+        <v>48</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>910</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1300</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-390</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>186</v>
+      </c>
+      <c r="C36" s="18">
+        <v>572</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-386</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>615</v>
+      </c>
+      <c r="C37" s="21">
+        <v>489</v>
+      </c>
+      <c r="D37" s="21">
+        <v>126</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>46</v>
+      </c>
+      <c r="C38" s="18">
+        <v>186</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-140</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>35</v>
+      </c>
+      <c r="C39" s="25">
+        <v>109</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-74</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="25">
+        <v>59</v>
+      </c>
+      <c r="C40" s="25">
+        <v>147</v>
+      </c>
+      <c r="D40" s="25">
+        <v>-88</v>
+      </c>
       <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="F40" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>20</v>
+      </c>
+      <c r="C41" s="25">
+        <v>41</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-21</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="25">
+        <v>8</v>
+      </c>
+      <c r="C42" s="25">
+        <v>56</v>
+      </c>
+      <c r="D42" s="25">
+        <v>-48</v>
+      </c>
       <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="F42" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0</v>
+      </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="9"/>
@@ -5023,133 +5446,253 @@
       <c r="A44" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="B44" s="21">
+        <v>98</v>
+      </c>
+      <c r="C44" s="21">
+        <v>103</v>
+      </c>
+      <c r="D44" s="21">
+        <v>-5</v>
+      </c>
       <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="F44" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>43</v>
+      </c>
+      <c r="C45" s="18">
+        <v>194</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-151</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="29"/>
+      <c r="B46" s="21">
+        <v>626</v>
+      </c>
+      <c r="C46" s="21">
+        <v>624</v>
+      </c>
+      <c r="D46" s="21">
+        <v>2</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="G46" s="5" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>1154</v>
+      </c>
+      <c r="C47" s="18">
+        <v>635</v>
+      </c>
+      <c r="D47" s="18">
+        <v>519</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>242</v>
+      </c>
+      <c r="C48" s="21">
+        <v>618</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-376</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>621</v>
+      </c>
+      <c r="C49" s="18">
+        <v>270</v>
+      </c>
+      <c r="D49" s="18">
+        <v>351</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>807</v>
+      </c>
+      <c r="C50" s="21">
+        <v>565</v>
+      </c>
+      <c r="D50" s="21">
+        <v>242</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="18">
+        <v>268</v>
+      </c>
+      <c r="C51" s="18">
+        <v>167</v>
+      </c>
+      <c r="D51" s="18">
+        <v>101</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="B52" s="21">
+        <v>374</v>
+      </c>
+      <c r="C52" s="21">
+        <v>449</v>
+      </c>
+      <c r="D52" s="21">
+        <v>-75</v>
+      </c>
       <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="18">
+        <v>203</v>
+      </c>
+      <c r="C53" s="18">
+        <v>241</v>
+      </c>
+      <c r="D53" s="18">
+        <v>-38</v>
+      </c>
       <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>51</v>
+      </c>
+      <c r="C54" s="21">
+        <v>257</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-206</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="27">
+        <v>407</v>
+      </c>
+      <c r="C55" s="27">
+        <v>196</v>
+      </c>
+      <c r="D55" s="27">
+        <v>211</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>263</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>

</xml_diff>

<commit_message>
Full statistic update for November 2024
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2024/2024_99_g_net_borrower_lender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DFBEBF-063E-4058-9F3B-639F86FC816A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE865377-F646-4F52-A885-ECD43DD0EFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="272">
   <si>
     <t>NET</t>
   </si>
@@ -853,6 +853,30 @@
   </si>
   <si>
     <t>2.08 : 1</t>
+  </si>
+  <si>
+    <t>0.24 : 1</t>
+  </si>
+  <si>
+    <t>2.00 : 1</t>
+  </si>
+  <si>
+    <t>1.55 : 1</t>
+  </si>
+  <si>
+    <t>0.77 : 1</t>
+  </si>
+  <si>
+    <t>2.62 : 1</t>
+  </si>
+  <si>
+    <t>0.97 : 1</t>
+  </si>
+  <si>
+    <t>0.16 : 1</t>
+  </si>
+  <si>
+    <t>3.61 : 1</t>
   </si>
 </sst>
 </file>
@@ -1762,15 +1786,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>14389</v>
+        <v>15885</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>12130</v>
+        <v>13212</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>2259</v>
+        <v>2673</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1782,7 +1806,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f t="shared" ref="G2:G33" si="2">IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.19 : 1</v>
+        <v>1.2 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1791,15 +1815,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>6346</v>
+        <v>6847</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>4332</v>
+        <v>4685</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>2014</v>
+        <v>2162</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1820,15 +1844,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>11795</v>
+        <v>12883</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>11967</v>
+        <v>13148</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>-172</v>
+        <v>-265</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1840,7 +1864,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.99 : 1</v>
+        <v>0.98 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1849,15 +1873,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>434</v>
+        <v>474</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>1279</v>
+        <v>1386</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-845</v>
+        <v>-912</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1878,15 +1902,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>10736</v>
+        <v>11635</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>14346</v>
+        <v>15664</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-3610</v>
+        <v>-4029</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1898,7 +1922,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.75 : 1</v>
+        <v>0.74 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1907,15 +1931,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>2772</v>
+        <v>2900</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>1675</v>
+        <v>1836</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>1097</v>
+        <v>1064</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1927,7 +1951,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.65 : 1</v>
+        <v>1.58 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1936,15 +1960,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>1338</v>
+        <v>1471</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>1905</v>
+        <v>2090</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-567</v>
+        <v>-619</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1965,15 +1989,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>448</v>
+        <v>477</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>709</v>
+        <v>768</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-261</v>
+        <v>-291</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1985,7 +2009,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.63 : 1</v>
+        <v>0.62 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1994,15 +2018,15 @@
       </c>
       <c r="B10" s="2">
         <f>January!B10+February!B10+March!B10+April!B10+May!B10+June!B10+July!B10+August!B10+September!B10+October!B10+November!B10+December!B10</f>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>503</v>
+        <v>544</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-484</v>
+        <v>-520</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2052,15 +2076,15 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2072,7 +2096,7 @@
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.63 : 1</v>
+        <v>1.55 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2081,15 +2105,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>1430</v>
+        <v>1505</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>825</v>
+        <v>866</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>605</v>
+        <v>639</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2101,7 +2125,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.73 : 1</v>
+        <v>1.74 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2110,15 +2134,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>1396</v>
+        <v>1596</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>2521</v>
+        <v>2724</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-1125</v>
+        <v>-1128</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2130,7 +2154,7 @@
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.55 : 1</v>
+        <v>0.59 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2139,15 +2163,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>613</v>
+        <v>661</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>1424</v>
+        <v>1542</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-811</v>
+        <v>-881</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2168,15 +2192,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>607</v>
+        <v>644</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1463</v>
+        <v>1602</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-856</v>
+        <v>-958</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2188,7 +2212,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.41 : 1</v>
+        <v>0.4 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2197,15 +2221,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>6070</v>
+        <v>6622</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>4200</v>
+        <v>4550</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>1870</v>
+        <v>2072</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2217,7 +2241,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.45 : 1</v>
+        <v>1.46 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2226,15 +2250,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>771</v>
+        <v>858</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>1081</v>
+        <v>1172</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-310</v>
+        <v>-314</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2246,7 +2270,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.71 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2255,15 +2279,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>5451</v>
+        <v>5895</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>4406</v>
+        <v>4719</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>1045</v>
+        <v>1176</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2275,7 +2299,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.24 : 1</v>
+        <v>1.25 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2284,15 +2308,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>742</v>
+        <v>791</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-607</v>
+        <v>-619</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2304,7 +2328,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.18 : 1</v>
+        <v>0.22 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2313,15 +2337,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>4966</v>
+        <v>5466</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>3521</v>
+        <v>3792</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>1445</v>
+        <v>1674</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2333,7 +2357,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.41 : 1</v>
+        <v>1.44 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2342,15 +2366,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>287</v>
+        <v>320</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>1118</v>
+        <v>1257</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-831</v>
+        <v>-937</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2362,7 +2386,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.26 : 1</v>
+        <v>0.25 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2371,15 +2395,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>6542</v>
+        <v>7017</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>3563</v>
+        <v>3801</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>2979</v>
+        <v>3216</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2391,7 +2415,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.84 : 1</v>
+        <v>1.85 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2400,15 +2424,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>16658</v>
+        <v>17995</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>11993</v>
+        <v>12974</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>4665</v>
+        <v>5021</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2429,15 +2453,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>1474</v>
+        <v>1640</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>3875</v>
+        <v>4348</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-2401</v>
+        <v>-2708</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2487,15 +2511,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>2413</v>
+        <v>2627</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>2019</v>
+        <v>2186</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>394</v>
+        <v>441</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2516,15 +2540,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>892</v>
+        <v>1004</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>955</v>
+        <v>1036</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-63</v>
+        <v>-32</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2536,7 +2560,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.93 : 1</v>
+        <v>0.97 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2545,15 +2569,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>5546</v>
+        <v>6207</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>4259</v>
+        <v>4726</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>1287</v>
+        <v>1481</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2565,7 +2589,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.3 : 1</v>
+        <v>1.31 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2574,15 +2598,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>438</v>
+        <v>451</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>224</v>
+        <v>262</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2594,7 +2618,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.96 : 1</v>
+        <v>1.72 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2603,15 +2627,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>2903</v>
+        <v>3141</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-2350</v>
+        <v>-2525</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2623,7 +2647,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.19 : 1</v>
+        <v>0.2 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2632,15 +2656,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>4294</v>
+        <v>4731</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>5640</v>
+        <v>6128</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-1346</v>
+        <v>-1397</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2652,7 +2676,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.76 : 1</v>
+        <v>0.77 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2661,15 +2685,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>3567</v>
+        <v>3821</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>5617</v>
+        <v>6071</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-2050</v>
+        <v>-2250</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2681,7 +2705,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.64 : 1</v>
+        <v>0.63 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2690,15 +2714,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>1760</v>
+        <v>1908</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>1043</v>
+        <v>1192</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E55" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -2710,7 +2734,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G55" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.69 : 1</v>
+        <v>1.6 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2719,15 +2743,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>8509</v>
+        <v>9364</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>11380</v>
+        <v>12411</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-2871</v>
+        <v>-3047</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2748,15 +2772,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>1932</v>
+        <v>2065</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>4846</v>
+        <v>5357</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-2914</v>
+        <v>-3292</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2768,7 +2792,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.4 : 1</v>
+        <v>0.39 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2777,15 +2801,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>4888</v>
+        <v>5350</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>3456</v>
+        <v>3755</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1432</v>
+        <v>1595</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2797,7 +2821,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.41 : 1</v>
+        <v>1.42 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2806,15 +2830,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>297</v>
+        <v>328</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>1770</v>
+        <v>1905</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-1473</v>
+        <v>-1577</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2835,15 +2859,15 @@
       </c>
       <c r="B39" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>796</v>
+        <v>880</v>
       </c>
       <c r="C39" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>799</v>
+        <v>885</v>
       </c>
       <c r="D39" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2855,7 +2879,7 @@
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1 : 1</v>
+        <v>0.99 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2864,15 +2888,15 @@
       </c>
       <c r="B40" s="8">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="C40" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>742</v>
+        <v>839</v>
       </c>
       <c r="D40" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-512</v>
+        <v>-591</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2884,7 +2908,7 @@
       </c>
       <c r="G40" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.31 : 1</v>
+        <v>0.3 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2893,15 +2917,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>465</v>
+        <v>574</v>
       </c>
       <c r="C41" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>825</v>
+        <v>947</v>
       </c>
       <c r="D41" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-360</v>
+        <v>-373</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2913,7 +2937,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.56 : 1</v>
+        <v>0.61 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2922,15 +2946,15 @@
       </c>
       <c r="B42" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C42" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>277</v>
+        <v>309</v>
       </c>
       <c r="D42" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-213</v>
+        <v>-229</v>
       </c>
       <c r="E42" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2942,7 +2966,7 @@
       </c>
       <c r="G42" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.23 : 1</v>
+        <v>0.26 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2951,15 +2975,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C43" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="D43" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-181</v>
+        <v>-199</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2971,7 +2995,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.24 : 1</v>
+        <v>0.25 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3009,15 +3033,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>772</v>
+        <v>824</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>1775</v>
+        <v>1968</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-1003</v>
+        <v>-1144</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3029,7 +3053,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.43 : 1</v>
+        <v>0.42 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3038,15 +3062,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>5267</v>
+        <v>5684</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>5825</v>
+        <v>6366</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-558</v>
+        <v>-682</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3058,7 +3082,7 @@
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.9 : 1</v>
+        <v>0.89 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3067,15 +3091,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>10574</v>
+        <v>11431</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>5821</v>
+        <v>6376</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>4753</v>
+        <v>5055</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3087,7 +3111,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.82 : 1</v>
+        <v>1.79 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3096,15 +3120,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>2495</v>
+        <v>2667</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>5804</v>
+        <v>6382</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-3309</v>
+        <v>-3715</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3116,7 +3140,7 @@
       </c>
       <c r="G48" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.43 : 1</v>
+        <v>0.42 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3125,15 +3149,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>5676</v>
+        <v>6336</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>2613</v>
+        <v>2865</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>3063</v>
+        <v>3471</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3145,7 +3169,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.17 : 1</v>
+        <v>2.21 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3154,15 +3178,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>9244</v>
+        <v>9934</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>5630</v>
+        <v>6154</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>3614</v>
+        <v>3780</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3174,7 +3198,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.64 : 1</v>
+        <v>1.61 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3183,15 +3207,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>2214</v>
+        <v>2405</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>1651</v>
+        <v>1812</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>563</v>
+        <v>593</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3203,7 +3227,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.34 : 1</v>
+        <v>1.33 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3212,15 +3236,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>3541</v>
+        <v>3853</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>4052</v>
+        <v>4374</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-511</v>
+        <v>-521</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3232,7 +3256,7 @@
       </c>
       <c r="G52" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.87 : 1</v>
+        <v>0.88 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3241,15 +3265,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>1371</v>
+        <v>1604</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>2296</v>
+        <v>2473</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-925</v>
+        <v>-869</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3261,7 +3285,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.6 : 1</v>
+        <v>0.65 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3270,15 +3294,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>284</v>
+        <v>322</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>2211</v>
+        <v>2442</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-1927</v>
+        <v>-2120</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3299,15 +3323,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>3268</v>
+        <v>3690</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>1960</v>
+        <v>2077</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>1308</v>
+        <v>1613</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3319,7 +3343,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>1.67 : 1</v>
+        <v>1.78 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -5722,7 +5746,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5762,108 +5786,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1496</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1082</v>
+      </c>
+      <c r="D2" s="18">
+        <v>414</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>501</v>
+      </c>
+      <c r="C3" s="21">
+        <v>353</v>
+      </c>
+      <c r="D3" s="21">
+        <v>148</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>1088</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1181</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-93</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>40</v>
+      </c>
+      <c r="C5" s="21">
+        <v>107</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-67</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>899</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1318</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-419</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="B7" s="21">
+        <v>128</v>
+      </c>
+      <c r="C7" s="21">
+        <v>161</v>
+      </c>
+      <c r="D7" s="21">
+        <v>-33</v>
+      </c>
       <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>133</v>
+      </c>
+      <c r="C8" s="18">
+        <v>185</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-52</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>29</v>
+      </c>
+      <c r="C9" s="21">
+        <v>59</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-30</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>5</v>
+      </c>
+      <c r="C10" s="18">
+        <v>41</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-36</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -5872,163 +5992,309 @@
       <c r="A12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="B12" s="23">
+        <v>11</v>
+      </c>
+      <c r="C12" s="23">
+        <v>18</v>
+      </c>
+      <c r="D12" s="23">
+        <v>-7</v>
+      </c>
       <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>75</v>
+      </c>
+      <c r="C13" s="23">
+        <v>41</v>
+      </c>
+      <c r="D13" s="23">
+        <v>34</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>200</v>
+      </c>
+      <c r="C14" s="23">
+        <v>203</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-3</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>48</v>
+      </c>
+      <c r="C15" s="23">
+        <v>118</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-70</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>37</v>
+      </c>
+      <c r="C16" s="18">
+        <v>139</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-102</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>552</v>
+      </c>
+      <c r="C17" s="21">
+        <v>350</v>
+      </c>
+      <c r="D17" s="21">
+        <v>202</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>87</v>
+      </c>
+      <c r="C18" s="18">
+        <v>91</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-4</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>444</v>
+      </c>
+      <c r="C19" s="21">
+        <v>313</v>
+      </c>
+      <c r="D19" s="21">
+        <v>131</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>37</v>
+      </c>
+      <c r="C20" s="18">
+        <v>49</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-12</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>500</v>
+      </c>
+      <c r="C21" s="21">
+        <v>271</v>
+      </c>
+      <c r="D21" s="21">
+        <v>229</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>33</v>
+      </c>
+      <c r="C22" s="18">
+        <v>139</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-106</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>475</v>
+      </c>
+      <c r="C23" s="21">
+        <v>238</v>
+      </c>
+      <c r="D23" s="21">
+        <v>237</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1337</v>
+      </c>
+      <c r="C24" s="18">
+        <v>981</v>
+      </c>
+      <c r="D24" s="18">
+        <v>356</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>166</v>
+      </c>
+      <c r="C25" s="21">
+        <v>473</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-307</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -6037,185 +6303,351 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>214</v>
+      </c>
+      <c r="C27" s="21">
+        <v>167</v>
+      </c>
+      <c r="D27" s="21">
+        <v>47</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="18">
+        <v>112</v>
+      </c>
+      <c r="C28" s="18">
+        <v>81</v>
+      </c>
+      <c r="D28" s="18">
+        <v>31</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>661</v>
+      </c>
+      <c r="C29" s="21">
+        <v>467</v>
+      </c>
+      <c r="D29" s="21">
+        <v>194</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="B30" s="18">
+        <v>13</v>
+      </c>
+      <c r="C30" s="18">
+        <v>38</v>
+      </c>
+      <c r="D30" s="18">
+        <v>-25</v>
+      </c>
       <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>63</v>
+      </c>
+      <c r="C31" s="21">
+        <v>238</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-175</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>437</v>
+      </c>
+      <c r="C32" s="18">
+        <v>488</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-51</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>254</v>
+      </c>
+      <c r="C33" s="21">
+        <v>454</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-200</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
+      <c r="B34" s="18">
+        <v>148</v>
+      </c>
+      <c r="C34" s="18">
+        <v>149</v>
+      </c>
+      <c r="D34" s="18">
+        <v>-1</v>
+      </c>
       <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="F34" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>855</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1031</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-176</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>133</v>
+      </c>
+      <c r="C36" s="18">
+        <v>511</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-378</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>462</v>
+      </c>
+      <c r="C37" s="21">
+        <v>299</v>
+      </c>
+      <c r="D37" s="21">
+        <v>163</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>31</v>
+      </c>
+      <c r="C38" s="18">
+        <v>135</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-104</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>18</v>
+      </c>
+      <c r="C39" s="25">
+        <v>97</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-79</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="25">
+        <v>109</v>
+      </c>
+      <c r="C40" s="25">
+        <v>122</v>
+      </c>
+      <c r="D40" s="25">
+        <v>-13</v>
+      </c>
       <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="F40" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>16</v>
+      </c>
+      <c r="C41" s="25">
+        <v>32</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-16</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="25">
+        <v>11</v>
+      </c>
+      <c r="C42" s="25">
+        <v>29</v>
+      </c>
+      <c r="D42" s="25">
+        <v>-18</v>
+      </c>
       <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="F42" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0</v>
+      </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="9"/>
@@ -6224,133 +6656,253 @@
       <c r="A44" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="B44" s="21">
+        <v>84</v>
+      </c>
+      <c r="C44" s="21">
+        <v>86</v>
+      </c>
+      <c r="D44" s="21">
+        <v>-2</v>
+      </c>
       <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="F44" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>52</v>
+      </c>
+      <c r="C45" s="18">
+        <v>193</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-141</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="B46" s="21">
+        <v>417</v>
+      </c>
+      <c r="C46" s="21">
+        <v>541</v>
+      </c>
+      <c r="D46" s="21">
+        <v>-124</v>
+      </c>
       <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="F46" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>857</v>
+      </c>
+      <c r="C47" s="18">
+        <v>555</v>
+      </c>
+      <c r="D47" s="18">
+        <v>302</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>172</v>
+      </c>
+      <c r="C48" s="21">
+        <v>578</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-406</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>660</v>
+      </c>
+      <c r="C49" s="18">
+        <v>252</v>
+      </c>
+      <c r="D49" s="18">
+        <v>408</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>690</v>
+      </c>
+      <c r="C50" s="21">
+        <v>524</v>
+      </c>
+      <c r="D50" s="21">
+        <v>166</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="18">
+        <v>191</v>
+      </c>
+      <c r="C51" s="18">
+        <v>161</v>
+      </c>
+      <c r="D51" s="18">
+        <v>30</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="B52" s="21">
+        <v>312</v>
+      </c>
+      <c r="C52" s="21">
+        <v>322</v>
+      </c>
+      <c r="D52" s="21">
+        <v>-10</v>
+      </c>
       <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="28"/>
+      <c r="B53" s="18">
+        <v>233</v>
+      </c>
+      <c r="C53" s="18">
+        <v>177</v>
+      </c>
+      <c r="D53" s="18">
+        <v>56</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="G53" s="3" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>38</v>
+      </c>
+      <c r="C54" s="21">
+        <v>231</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-193</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="27">
+        <v>422</v>
+      </c>
+      <c r="C55" s="27">
+        <v>117</v>
+      </c>
+      <c r="D55" s="27">
+        <v>305</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>271</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>

</xml_diff>

<commit_message>
Update December 2024 statistics
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2024/2024_99_g_net_borrower_lender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE865377-F646-4F52-A885-ECD43DD0EFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D4AC52-B5B3-4BED-A19C-7741B16CE70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="282">
   <si>
     <t>NET</t>
   </si>
@@ -877,6 +877,36 @@
   </si>
   <si>
     <t>3.61 : 1</t>
+  </si>
+  <si>
+    <t>1.12 : 1</t>
+  </si>
+  <si>
+    <t>0.91 : 1</t>
+  </si>
+  <si>
+    <t>1.29 : 1</t>
+  </si>
+  <si>
+    <t>0.29 : 1</t>
+  </si>
+  <si>
+    <t>1.22 : 1</t>
+  </si>
+  <si>
+    <t>1.52 : 1</t>
+  </si>
+  <si>
+    <t>3.53 : 1</t>
+  </si>
+  <si>
+    <t>1.65 : 1</t>
+  </si>
+  <si>
+    <t>0.94 : 1</t>
+  </si>
+  <si>
+    <t>3.58 : 1</t>
   </si>
 </sst>
 </file>
@@ -1786,15 +1816,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>15885</v>
+        <v>17209</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>13212</v>
+        <v>14314</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>2673</v>
+        <v>2895</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -1815,15 +1845,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>6847</v>
+        <v>7357</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>4685</v>
+        <v>5054</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>2162</v>
+        <v>2303</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1844,15 +1874,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>12883</v>
+        <v>13858</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>13148</v>
+        <v>14246</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>-265</v>
+        <v>-388</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1864,7 +1894,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.98 : 1</v>
+        <v>0.97 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1873,15 +1903,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>474</v>
+        <v>503</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>1386</v>
+        <v>1490</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-912</v>
+        <v>-987</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1902,15 +1932,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>11635</v>
+        <v>12471</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>15664</v>
+        <v>17039</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-4029</v>
+        <v>-4568</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1922,7 +1952,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.74 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1931,15 +1961,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>2900</v>
+        <v>3054</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>1836</v>
+        <v>1994</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -1951,7 +1981,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.58 : 1</v>
+        <v>1.53 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1960,15 +1990,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>1471</v>
+        <v>1611</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>2090</v>
+        <v>2233</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-619</v>
+        <v>-622</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1980,7 +2010,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.7 : 1</v>
+        <v>0.72 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1989,15 +2019,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>477</v>
+        <v>509</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>768</v>
+        <v>817</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-291</v>
+        <v>-308</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2018,15 +2048,15 @@
       </c>
       <c r="B10" s="2">
         <f>January!B10+February!B10+March!B10+April!B10+May!B10+June!B10+July!B10+August!B10+September!B10+October!B10+November!B10+December!B10</f>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>544</v>
+        <v>570</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-520</v>
+        <v>-543</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2038,7 +2068,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.04 : 1</v>
+        <v>0.05 : 1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2076,15 +2106,15 @@
       </c>
       <c r="B12" s="6">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>340</v>
+        <v>359</v>
       </c>
       <c r="C12" s="6">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="D12" s="6">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E12" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2096,7 +2126,7 @@
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.55 : 1</v>
+        <v>1.51 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2105,15 +2135,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>1505</v>
+        <v>1596</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>866</v>
+        <v>920</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>639</v>
+        <v>676</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2125,7 +2155,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.74 : 1</v>
+        <v>1.73 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2134,15 +2164,15 @@
       </c>
       <c r="B14" s="6">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>1596</v>
+        <v>1740</v>
       </c>
       <c r="C14" s="6">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>2724</v>
+        <v>2883</v>
       </c>
       <c r="D14" s="6">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-1128</v>
+        <v>-1143</v>
       </c>
       <c r="E14" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2154,7 +2184,7 @@
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.59 : 1</v>
+        <v>0.6 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2163,15 +2193,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>661</v>
+        <v>704</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>1542</v>
+        <v>1675</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-881</v>
+        <v>-971</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -2183,7 +2213,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.43 : 1</v>
+        <v>0.42 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2192,15 +2222,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>644</v>
+        <v>708</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1602</v>
+        <v>1749</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-958</v>
+        <v>-1041</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2221,15 +2251,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>6622</v>
+        <v>7121</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>4550</v>
+        <v>4937</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>2072</v>
+        <v>2184</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2241,7 +2271,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.46 : 1</v>
+        <v>1.44 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2250,15 +2280,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>858</v>
+        <v>922</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>1172</v>
+        <v>1233</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-314</v>
+        <v>-311</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2270,7 +2300,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.73 : 1</v>
+        <v>0.75 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2279,15 +2309,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>5895</v>
+        <v>6322</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>4719</v>
+        <v>5063</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>1176</v>
+        <v>1259</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2308,15 +2338,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>791</v>
+        <v>829</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-619</v>
+        <v>-637</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2328,7 +2358,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.22 : 1</v>
+        <v>0.23 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2337,15 +2367,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>5466</v>
+        <v>5943</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>3792</v>
+        <v>4052</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>1674</v>
+        <v>1891</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2357,7 +2387,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.44 : 1</v>
+        <v>1.47 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2366,15 +2396,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>320</v>
+        <v>365</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>1257</v>
+        <v>1410</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-937</v>
+        <v>-1045</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2386,7 +2416,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.25 : 1</v>
+        <v>0.26 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2395,15 +2425,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>7017</v>
+        <v>7484</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>3801</v>
+        <v>4065</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>3216</v>
+        <v>3419</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2415,7 +2445,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.85 : 1</v>
+        <v>1.84 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2424,15 +2454,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>17995</v>
+        <v>19415</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>12974</v>
+        <v>14034</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>5021</v>
+        <v>5381</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2444,7 +2474,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.39 : 1</v>
+        <v>1.38 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2453,15 +2483,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>1640</v>
+        <v>1817</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>4348</v>
+        <v>4745</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-2708</v>
+        <v>-2928</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2511,15 +2541,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>2627</v>
+        <v>2854</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>2186</v>
+        <v>2333</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>441</v>
+        <v>521</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2531,7 +2561,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.2 : 1</v>
+        <v>1.22 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2540,15 +2570,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>1004</v>
+        <v>1077</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>1036</v>
+        <v>1123</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>-32</v>
+        <v>-46</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2560,7 +2590,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.97 : 1</v>
+        <v>0.96 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2569,15 +2599,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>6207</v>
+        <v>6746</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>4726</v>
+        <v>5167</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>1481</v>
+        <v>1579</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2598,15 +2628,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>451</v>
+        <v>506</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2618,7 +2648,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.72 : 1</v>
+        <v>1.74 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2627,15 +2657,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>616</v>
+        <v>663</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>3141</v>
+        <v>3312</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-2525</v>
+        <v>-2649</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2656,15 +2686,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>4731</v>
+        <v>5085</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>6128</v>
+        <v>6631</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-1397</v>
+        <v>-1546</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -2685,15 +2715,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>3821</v>
+        <v>4143</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>6071</v>
+        <v>6498</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-2250</v>
+        <v>-2355</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -2705,7 +2735,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.63 : 1</v>
+        <v>0.64 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2714,15 +2744,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>1908</v>
+        <v>2086</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>1192</v>
+        <v>1309</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>716</v>
+        <v>777</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E55" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -2734,7 +2764,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G55" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.6 : 1</v>
+        <v>1.59 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2743,15 +2773,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>9364</v>
+        <v>10096</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>12411</v>
+        <v>13408</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-3047</v>
+        <v>-3312</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2772,15 +2802,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>2065</v>
+        <v>2188</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>5357</v>
+        <v>5796</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-3292</v>
+        <v>-3608</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2792,7 +2822,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.39 : 1</v>
+        <v>0.38 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2801,15 +2831,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>5350</v>
+        <v>5834</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>3755</v>
+        <v>4063</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1595</v>
+        <v>1771</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2821,7 +2851,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.42 : 1</v>
+        <v>1.44 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2830,15 +2860,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>328</v>
+        <v>359</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>1905</v>
+        <v>2034</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-1577</v>
+        <v>-1675</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -2850,7 +2880,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.17 : 1</v>
+        <v>0.18 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2859,15 +2889,15 @@
       </c>
       <c r="B39" s="4">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>880</v>
+        <v>954</v>
       </c>
       <c r="C39" s="4">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>885</v>
+        <v>960</v>
       </c>
       <c r="D39" s="4">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -2888,15 +2918,15 @@
       </c>
       <c r="B40" s="8">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>248</v>
+        <v>269</v>
       </c>
       <c r="C40" s="8">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>839</v>
+        <v>919</v>
       </c>
       <c r="D40" s="8">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-591</v>
+        <v>-650</v>
       </c>
       <c r="E40" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2908,7 +2938,7 @@
       </c>
       <c r="G40" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.3 : 1</v>
+        <v>0.29 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2917,15 +2947,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>574</v>
+        <v>662</v>
       </c>
       <c r="C41" s="8">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>947</v>
+        <v>1093</v>
       </c>
       <c r="D41" s="8">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-373</v>
+        <v>-431</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2946,15 +2976,15 @@
       </c>
       <c r="B42" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C42" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>309</v>
+        <v>335</v>
       </c>
       <c r="D42" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-229</v>
+        <v>-252</v>
       </c>
       <c r="E42" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2966,7 +2996,7 @@
       </c>
       <c r="G42" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.26 : 1</v>
+        <v>0.25 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2975,15 +3005,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C43" s="8">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>267</v>
+        <v>290</v>
       </c>
       <c r="D43" s="8">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-199</v>
+        <v>-216</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -2995,7 +3025,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.25 : 1</v>
+        <v>0.26 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3033,15 +3063,15 @@
       </c>
       <c r="B45" s="2">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>824</v>
+        <v>887</v>
       </c>
       <c r="C45" s="2">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>1968</v>
+        <v>2139</v>
       </c>
       <c r="D45" s="2">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-1144</v>
+        <v>-1252</v>
       </c>
       <c r="E45" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3053,7 +3083,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.42 : 1</v>
+        <v>0.41 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3062,15 +3092,15 @@
       </c>
       <c r="B46" s="4">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>5684</v>
+        <v>6083</v>
       </c>
       <c r="C46" s="4">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>6366</v>
+        <v>6755</v>
       </c>
       <c r="D46" s="4">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>-682</v>
+        <v>-672</v>
       </c>
       <c r="E46" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3082,7 +3112,7 @@
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.89 : 1</v>
+        <v>0.9 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3091,15 +3121,15 @@
       </c>
       <c r="B47" s="2">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>11431</v>
+        <v>12223</v>
       </c>
       <c r="C47" s="2">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>6376</v>
+        <v>6882</v>
       </c>
       <c r="D47" s="2">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>5055</v>
+        <v>5341</v>
       </c>
       <c r="E47" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3111,7 +3141,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.79 : 1</v>
+        <v>1.78 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3120,15 +3150,15 @@
       </c>
       <c r="B48" s="4">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>2667</v>
+        <v>2822</v>
       </c>
       <c r="C48" s="4">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>6382</v>
+        <v>6919</v>
       </c>
       <c r="D48" s="4">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>-3715</v>
+        <v>-4097</v>
       </c>
       <c r="E48" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3140,7 +3170,7 @@
       </c>
       <c r="G48" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.42 : 1</v>
+        <v>0.41 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3149,15 +3179,15 @@
       </c>
       <c r="B49" s="2">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>6336</v>
+        <v>6986</v>
       </c>
       <c r="C49" s="2">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>2865</v>
+        <v>3049</v>
       </c>
       <c r="D49" s="2">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>3471</v>
+        <v>3937</v>
       </c>
       <c r="E49" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3169,7 +3199,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.21 : 1</v>
+        <v>2.29 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3178,15 +3208,15 @@
       </c>
       <c r="B50" s="4">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>9934</v>
+        <v>10711</v>
       </c>
       <c r="C50" s="4">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>6154</v>
+        <v>6625</v>
       </c>
       <c r="D50" s="4">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>3780</v>
+        <v>4086</v>
       </c>
       <c r="E50" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3198,7 +3228,7 @@
       </c>
       <c r="G50" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.61 : 1</v>
+        <v>1.62 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3207,15 +3237,15 @@
       </c>
       <c r="B51" s="2">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>2405</v>
+        <v>2566</v>
       </c>
       <c r="C51" s="2">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>1812</v>
+        <v>1983</v>
       </c>
       <c r="D51" s="2">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="E51" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3227,7 +3257,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.33 : 1</v>
+        <v>1.29 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3236,15 +3266,15 @@
       </c>
       <c r="B52" s="4">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>3853</v>
+        <v>4062</v>
       </c>
       <c r="C52" s="4">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>4374</v>
+        <v>4600</v>
       </c>
       <c r="D52" s="4">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-521</v>
+        <v>-538</v>
       </c>
       <c r="E52" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3265,15 +3295,15 @@
       </c>
       <c r="B53" s="2">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>1604</v>
+        <v>1736</v>
       </c>
       <c r="C53" s="2">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>2473</v>
+        <v>2638</v>
       </c>
       <c r="D53" s="2">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-869</v>
+        <v>-902</v>
       </c>
       <c r="E53" s="28" t="str">
         <f t="shared" si="3"/>
@@ -3285,7 +3315,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.65 : 1</v>
+        <v>0.66 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3294,15 +3324,15 @@
       </c>
       <c r="B54" s="4">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>322</v>
+        <v>352</v>
       </c>
       <c r="C54" s="4">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>2442</v>
+        <v>2639</v>
       </c>
       <c r="D54" s="4">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>-2120</v>
+        <v>-2287</v>
       </c>
       <c r="E54" s="29" t="str">
         <f t="shared" si="3"/>
@@ -3323,15 +3353,15 @@
       </c>
       <c r="B55" s="10">
         <f>January!B55+February!B55+March!B55+April!B55+May!B55+June!B55+July!B55+August!B55+September!B55+October!B55+November!B55+December!B55</f>
-        <v>3690</v>
+        <v>4209</v>
       </c>
       <c r="C55" s="10">
         <f>January!C55+February!C55+March!C55+April!C55+May!C55+June!C55+July!C55+August!C55+September!C55+October!C55+November!C55+December!C55</f>
-        <v>2077</v>
+        <v>2222</v>
       </c>
       <c r="D55" s="10">
         <f>January!D55+February!D55+March!D55+April!D55+May!D55+June!D55+July!D55+August!D55+September!D55+October!D55+November!D55+December!D55</f>
-        <v>1613</v>
+        <v>1987</v>
       </c>
       <c r="E55" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3343,7 +3373,7 @@
       </c>
       <c r="G55" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>1.78 : 1</v>
+        <v>1.89 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -6934,7 +6964,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6974,108 +7004,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1324</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1102</v>
+      </c>
+      <c r="D2" s="18">
+        <v>222</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>510</v>
+      </c>
+      <c r="C3" s="21">
+        <v>369</v>
+      </c>
+      <c r="D3" s="21">
+        <v>141</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>975</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1098</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-123</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>29</v>
+      </c>
+      <c r="C5" s="21">
+        <v>104</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-75</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>836</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1375</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-539</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="B7" s="21">
+        <v>154</v>
+      </c>
+      <c r="C7" s="21">
+        <v>158</v>
+      </c>
+      <c r="D7" s="21">
+        <v>-4</v>
+      </c>
       <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>140</v>
+      </c>
+      <c r="C8" s="18">
+        <v>143</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-3</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>32</v>
+      </c>
+      <c r="C9" s="21">
+        <v>49</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-17</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>3</v>
+      </c>
+      <c r="C10" s="18">
+        <v>26</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-23</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -7084,163 +7210,309 @@
       <c r="A12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="30"/>
+      <c r="B12" s="23">
+        <v>19</v>
+      </c>
+      <c r="C12" s="23">
+        <v>17</v>
+      </c>
+      <c r="D12" s="23">
+        <v>2</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F12" s="30"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>91</v>
+      </c>
+      <c r="C13" s="23">
+        <v>54</v>
+      </c>
+      <c r="D13" s="23">
+        <v>37</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="23">
+        <v>144</v>
+      </c>
+      <c r="C14" s="23">
+        <v>159</v>
+      </c>
+      <c r="D14" s="23">
+        <v>-15</v>
+      </c>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>43</v>
+      </c>
+      <c r="C15" s="23">
+        <v>133</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-90</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>64</v>
+      </c>
+      <c r="C16" s="18">
+        <v>147</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-83</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>499</v>
+      </c>
+      <c r="C17" s="21">
+        <v>387</v>
+      </c>
+      <c r="D17" s="21">
+        <v>112</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="18">
+        <v>64</v>
+      </c>
+      <c r="C18" s="18">
+        <v>61</v>
+      </c>
+      <c r="D18" s="18">
+        <v>3</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>427</v>
+      </c>
+      <c r="C19" s="21">
+        <v>344</v>
+      </c>
+      <c r="D19" s="21">
+        <v>83</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>20</v>
+      </c>
+      <c r="C20" s="18">
+        <v>38</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-18</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>477</v>
+      </c>
+      <c r="C21" s="21">
+        <v>260</v>
+      </c>
+      <c r="D21" s="21">
+        <v>217</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>45</v>
+      </c>
+      <c r="C22" s="18">
+        <v>153</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-108</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>467</v>
+      </c>
+      <c r="C23" s="21">
+        <v>264</v>
+      </c>
+      <c r="D23" s="21">
+        <v>203</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1420</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1060</v>
+      </c>
+      <c r="D24" s="18">
+        <v>360</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>177</v>
+      </c>
+      <c r="C25" s="21">
+        <v>397</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-220</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -7249,185 +7521,351 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>227</v>
+      </c>
+      <c r="C27" s="21">
+        <v>147</v>
+      </c>
+      <c r="D27" s="21">
+        <v>80</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="18">
+        <v>73</v>
+      </c>
+      <c r="C28" s="18">
+        <v>87</v>
+      </c>
+      <c r="D28" s="18">
+        <v>-14</v>
+      </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>539</v>
+      </c>
+      <c r="C29" s="21">
+        <v>441</v>
+      </c>
+      <c r="D29" s="21">
+        <v>98</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="18">
+        <v>55</v>
+      </c>
+      <c r="C30" s="18">
+        <v>28</v>
+      </c>
+      <c r="D30" s="18">
+        <v>27</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>47</v>
+      </c>
+      <c r="C31" s="21">
+        <v>171</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-124</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>354</v>
+      </c>
+      <c r="C32" s="18">
+        <v>503</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-149</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="21">
+        <v>322</v>
+      </c>
+      <c r="C33" s="21">
+        <v>427</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-105</v>
+      </c>
       <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="F33" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>178</v>
+      </c>
+      <c r="C34" s="18">
+        <v>117</v>
+      </c>
+      <c r="D34" s="18">
+        <v>61</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>732</v>
+      </c>
+      <c r="C35" s="21">
+        <v>997</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-265</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>123</v>
+      </c>
+      <c r="C36" s="18">
+        <v>439</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-316</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>484</v>
+      </c>
+      <c r="C37" s="21">
+        <v>308</v>
+      </c>
+      <c r="D37" s="21">
+        <v>176</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>31</v>
+      </c>
+      <c r="C38" s="18">
+        <v>129</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-98</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="B39" s="25">
+        <v>21</v>
+      </c>
+      <c r="C39" s="25">
+        <v>80</v>
+      </c>
+      <c r="D39" s="25">
+        <v>-59</v>
+      </c>
       <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="25">
+        <v>88</v>
+      </c>
+      <c r="C40" s="25">
+        <v>146</v>
+      </c>
+      <c r="D40" s="25">
+        <v>-58</v>
+      </c>
       <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="9"/>
+      <c r="F40" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>3</v>
+      </c>
+      <c r="C41" s="25">
+        <v>26</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-23</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="25">
+        <v>6</v>
+      </c>
+      <c r="C42" s="25">
+        <v>23</v>
+      </c>
+      <c r="D42" s="25">
+        <v>-17</v>
+      </c>
       <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="9"/>
+      <c r="F42" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>0</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0</v>
+      </c>
       <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="9"/>
@@ -7436,133 +7874,253 @@
       <c r="A44" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="B44" s="21">
+        <v>74</v>
+      </c>
+      <c r="C44" s="21">
+        <v>75</v>
+      </c>
+      <c r="D44" s="21">
+        <v>-1</v>
+      </c>
       <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="5"/>
+      <c r="F44" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="18">
+        <v>63</v>
+      </c>
+      <c r="C45" s="18">
+        <v>171</v>
+      </c>
+      <c r="D45" s="18">
+        <v>-108</v>
+      </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="29"/>
+      <c r="B46" s="21">
+        <v>399</v>
+      </c>
+      <c r="C46" s="21">
+        <v>389</v>
+      </c>
+      <c r="D46" s="21">
+        <v>10</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F46" s="29"/>
-      <c r="G46" s="5"/>
+      <c r="G46" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="18">
+        <v>792</v>
+      </c>
+      <c r="C47" s="18">
+        <v>506</v>
+      </c>
+      <c r="D47" s="18">
+        <v>286</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="21">
+        <v>155</v>
+      </c>
+      <c r="C48" s="21">
+        <v>537</v>
+      </c>
+      <c r="D48" s="21">
+        <v>-382</v>
+      </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="18">
+        <v>650</v>
+      </c>
+      <c r="C49" s="18">
+        <v>184</v>
+      </c>
+      <c r="D49" s="18">
+        <v>466</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="21">
+        <v>777</v>
+      </c>
+      <c r="C50" s="21">
+        <v>471</v>
+      </c>
+      <c r="D50" s="21">
+        <v>306</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
+      <c r="B51" s="18">
+        <v>161</v>
+      </c>
+      <c r="C51" s="18">
+        <v>171</v>
+      </c>
+      <c r="D51" s="18">
+        <v>-10</v>
+      </c>
       <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
+      <c r="F51" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="B52" s="21">
+        <v>209</v>
+      </c>
+      <c r="C52" s="21">
+        <v>226</v>
+      </c>
+      <c r="D52" s="21">
+        <v>-17</v>
+      </c>
       <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="18">
+        <v>132</v>
+      </c>
+      <c r="C53" s="18">
+        <v>165</v>
+      </c>
+      <c r="D53" s="18">
+        <v>-33</v>
+      </c>
       <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="21">
+        <v>30</v>
+      </c>
+      <c r="C54" s="21">
+        <v>197</v>
+      </c>
+      <c r="D54" s="21">
+        <v>-167</v>
+      </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="27">
+        <v>519</v>
+      </c>
+      <c r="C55" s="27">
+        <v>145</v>
+      </c>
+      <c r="D55" s="27">
+        <v>374</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F55" s="32"/>
-      <c r="G55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>281</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G55" xr:uid="{00000000-0009-0000-0000-00000C000000}"/>

</xml_diff>